<commit_message>
chore: sync latest changes - UI refinements and reservation collector updates
</commit_message>
<xml_diff>
--- a/통합 문서1.xlsx
+++ b/통합 문서1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjheu\Desktop\ERPcheck\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aeone\Desktop\ERPcheck\ERPcheck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1936873-032A-4223-BBBD-ECDF40C903D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294DA311-7C1D-4C49-B866-3F9C279E6336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="12900" xr2:uid="{68BE0DFE-6DEC-47F4-A8FB-1C51BE5473BB}"/>
+    <workbookView xWindow="15" yWindow="2085" windowWidth="28800" windowHeight="13425" xr2:uid="{68BE0DFE-6DEC-47F4-A8FB-1C51BE5473BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>상품 종류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>&lt;option value="20"&gt;dobong-1&lt;/option&gt;&lt;option value="21"&gt;dobong-2&lt;/option&gt;&lt;option value="22"&gt;dobong-3&lt;/option&gt;&lt;option value="24"&gt;dobong-5&lt;/option&gt;&lt;option value="25"&gt;dobong-6&lt;/option&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;label class="nullGoodsLabel" style="margin:5px 3px; width: 100%;"&gt;
+                                                &lt;input type="checkbox" class="nullGoods"&gt; 상품 없음
+                                            &lt;/label&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -224,9 +230,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -564,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9942FE54-9717-49DB-A04C-34DE9ECE2502}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -642,7 +651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -651,6 +660,9 @@
       </c>
       <c r="D5" t="s">
         <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="F5" t="s">
         <v>36</v>

</xml_diff>